<commit_message>
Speaker and Sponser File Name Changes
</commit_message>
<xml_diff>
--- a/Test Data/E2MDataImportTemplate.xlsx
+++ b/Test Data/E2MDataImportTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Session" sheetId="1" state="visible" r:id="rId2"/>
@@ -293,6 +293,58 @@
     <author> </author>
   </authors>
   <commentList>
+    <comment ref="D2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Web Spiders:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Mandatory Field; Please enter the name of the department or office the speaker belongs to; Character limit 100 including spaces.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Web Spiders:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Mandatory Field; Please enter the name of Company/Organisation/Institute/Consultancy the speaker belongs to; character limit 100 with spaces.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="F2" authorId="0">
       <text>
         <r>
@@ -315,7 +367,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Mandatory Field; Please enter the name of the department or office the speaker belongs to; Character limit 100 including spaces.</t>
+          <t xml:space="preserve">Optional field; Please enter the email address of Speaker or leave blank if not available.</t>
         </r>
       </text>
     </comment>
@@ -341,7 +393,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Mandatory Field; Please enter the name of Company/Organisation/Institute/Consultancy the speaker belongs to; character limit 100 with spaces.</t>
+          <t xml:space="preserve">Optional field. Enter the name of the city/town. Character count 100 with spaces</t>
         </r>
       </text>
     </comment>
@@ -367,7 +419,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Optional field; Please enter the email address of Speaker or leave blank if not available.</t>
+          <t xml:space="preserve">Optional field. Enter the name of the state/county or leave blank. Character count 100 with spaces</t>
         </r>
       </text>
     </comment>
@@ -393,7 +445,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Optional field. Enter the name of the city/town. Character count 100 with spaces</t>
+          <t xml:space="preserve">Optional field. Enter the name of the country. Enter the three letter Country acronym, e.g. USA/UAE/IND etc</t>
         </r>
       </text>
     </comment>
@@ -419,7 +471,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Optional field. Enter the name of the state/county or leave blank. Character count 100 with spaces</t>
+          <t xml:space="preserve">Optional field. Enter the Speaker bio information. You can provide paragraph breaks in the texts. Character limit 1200 including spaces.</t>
         </r>
       </text>
     </comment>
@@ -445,7 +497,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Optional field. Enter the name of the country. Enter the three letter Country acronym, e.g. USA/UAE/IND etc</t>
+          <t xml:space="preserve">Optional field. Enter the URL/link to the Facebook profile page of the speaker.</t>
         </r>
       </text>
     </comment>
@@ -471,7 +523,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Optional field. Enter the Speaker bio information. You can provide paragraph breaks in the texts. Character limit 1200 including spaces.</t>
+          <t xml:space="preserve">Optional field. Enter the URL/link to the Twitter profile page of the speaker.</t>
         </r>
       </text>
     </comment>
@@ -497,7 +549,8 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Optional field. Enter the URL/link to the Facebook profile page of the speaker.</t>
+          <t xml:space="preserve">Optional field. Enter the URL/link to the LinkedIn profile page of the speaker.
+</t>
         </r>
       </text>
     </comment>
@@ -523,64 +576,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Optional field. Enter the URL/link to the Twitter profile page of the speaker.</t>
+          <t xml:space="preserve">Optional field. Enter the name of the image file that needs to be associated with the speaker. The same image(with the filename) should be available in the assets.zip folder when you upload. Also note the Assets.zip folder should be created by selecting all files together, and the images shouldn't reside inside a folder and folder zipped. Image formats PNG/JPG in 72 dpi in dimension of 120x120 pixels; images should be in square dimension.</t>
         </r>
       </text>
     </comment>
     <comment ref="O2" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b val="true"/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Web Spiders:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Optional field. Enter the URL/link to the LinkedIn profile page of the speaker.
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="P2" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b val="true"/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Web Spiders:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Optional field. Enter the name of the image file that needs to be associated with the speaker. The same image(with the filename) should be available in the assets.zip folder when you upload. Also note the Assets.zip folder should be created by selecting all files together, and the images shouldn't reside inside a folder and folder zipped. Image formats PNG/JPG in 72 dpi in dimension of 120x120 pixels; images should be in square dimension.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="Q2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1754,149 +1754,147 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="C1:S3"/>
+  <dimension ref="A2:Q3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q3" activeCellId="0" sqref="Q3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="4.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="23.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="30.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="22.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="23.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="30.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="49.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="25.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="37.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="42.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="49.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="20" style="0" width="4.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="23.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="30.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="22.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="23.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="30.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="49.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="25.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="37.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="42.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="49.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="18" style="0" width="4.71"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="2" customFormat="false" ht="43.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>22</v>
+      </c>
       <c r="C2" s="10" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="M2" s="10" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="N2" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="O2" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="P2" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="O2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="R2" s="11" t="s">
+      <c r="P2" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="S2" s="11" t="s">
+      <c r="Q2" s="11" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>39</v>
+      </c>
       <c r="C3" s="9" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>43</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="H3" s="12" t="s">
-        <v>43</v>
+        <v>44</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>44</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="N3" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="O3" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="P3" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="Q3" s="13" t="s">
+      <c r="O3" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="R3" s="13" t="s">
+      <c r="P3" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="S3" s="14" t="s">
+      <c r="Q3" s="14" t="s">
         <v>52</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H3" r:id="rId2" display="anie@karak.com"/>
-    <hyperlink ref="M3" r:id="rId3" display="anie@facebook.com"/>
-    <hyperlink ref="N3" r:id="rId4" display="anie@twitter.com"/>
-    <hyperlink ref="O3" r:id="rId5" display="anie@linkedin.com"/>
-    <hyperlink ref="S3" r:id="rId6" display="https://aniekarak.com"/>
+    <hyperlink ref="F3" r:id="rId2" display="anie@karak.com"/>
+    <hyperlink ref="K3" r:id="rId3" display="anie@facebook.com"/>
+    <hyperlink ref="L3" r:id="rId4" display="anie@twitter.com"/>
+    <hyperlink ref="M3" r:id="rId5" display="anie@linkedin.com"/>
+    <hyperlink ref="Q3" r:id="rId6" display="https://aniekarak.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1953,8 +1951,8 @@
   </sheetPr>
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>